<commit_message>
Update MCKP results and readme
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenjunlin08/Documents/GitHub/CSCI596-Final-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenjunlin08/Documents/GitHub/CSCI596-Final-Project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D6BF16-3A2C-994B-B39A-CF57BE116F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5B26E1-96F3-C54C-813D-ADCE0F38E8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9380" yWindow="2380" windowWidth="28040" windowHeight="17440" xr2:uid="{272D8041-8F99-154B-B284-2900F66D7330}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="34680" windowHeight="21900" xr2:uid="{272D8041-8F99-154B-B284-2900F66D7330}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Plot" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="22">
   <si>
     <t>knapsack_baseline.out</t>
   </si>
@@ -89,6 +90,18 @@
   </si>
   <si>
     <t>Std</t>
+  </si>
+  <si>
+    <t>n=1,000,000</t>
+  </si>
+  <si>
+    <t>n=10,000,000</t>
+  </si>
+  <si>
+    <t>n=100,000,000</t>
+  </si>
+  <si>
+    <t>MCKP_mpi.out</t>
   </si>
 </sst>
 </file>
@@ -157,6 +170,3407 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Running Time Results of the Lagrangian-dual-based algorithm with MPI implementation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plot!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=1,000,000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Plot!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29333333333333328</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9141-5F42-8FF4-7163C8061825}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plot!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=10,000,000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Plot!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.6733333333333329</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1233333333333335</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1366666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9141-5F42-8FF4-7163C8061825}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plot!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=100,000,000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Plot!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>41.593333333333334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.926666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.243333333333336</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9141-5F42-8FF4-7163C8061825}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="481588544"/>
+        <c:axId val="481590544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="481588544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Num. Processors</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481590544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="481590544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Running Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481588544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fixed Problem-Size Scaling</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Results </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>of the Lagrangian-dual-based algorithm with MPI implementation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plot!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=1,000,000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Plot!$F$2:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88732394366197176</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72413793103448276</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35795454545454553</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-66CE-7649-9E87-4FF9495318EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plot!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=10,000,000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Plot!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89203354297693904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.66797488226059643</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3319032761310452</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-66CE-7649-9E87-4FF9495318EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plot!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=100,000,000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Plot!$H$2:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8343139876972453</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52971642044489731</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24474344892515296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-66CE-7649-9E87-4FF9495318EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="481588544"/>
+        <c:axId val="481590544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="481588544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Num. Processors</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481590544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="481590544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481588544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fixed Problem-Size Scaling</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Results </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>of the Lagrangian-dual-based algorithm with MPI implementation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plot!$F$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=1,000,000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Plot!$F$28:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68555900621118004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36914715719063546</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28893979057591623</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BBBA-1443-972C-903345544171}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plot!$G$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=10,000,000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Plot!$G$28:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61181533646322372</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3246553728616508</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26063333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BBBA-1443-972C-903345544171}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="481588544"/>
+        <c:axId val="481590544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="481588544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Num. Processors</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481590544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="481590544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481588544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>69851</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>436880</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>59690</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13DE66C5-EA5A-C5BF-635A-0A297CB60F09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>255269</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>97790</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DA70078-F733-4641-AFCC-1424A293B09B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>741680</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>712469</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0855B4E3-9436-1944-BE5E-2528486C9225}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,10 +3870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC87B85-F8B1-9F4E-A67F-15AC1BD6B5C6}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="159" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="118" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1697,7 +5111,7 @@
         <v>5.010402512107512</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>100000000</v>
       </c>
@@ -1714,7 +5128,7 @@
         <v>101.22</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>100000000</v>
       </c>
@@ -1731,7 +5145,7 @@
         <v>101.53</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>100000000</v>
       </c>
@@ -1748,7 +5162,7 @@
         <v>148.69</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
         <v>16</v>
       </c>
@@ -1765,7 +5179,7 @@
         <v>117.14666666666666</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
         <v>17</v>
       </c>
@@ -1782,7 +5196,491 @@
         <v>27.317767722369499</v>
       </c>
     </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1000000</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>3.01</v>
+      </c>
+      <c r="D57">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E57">
+        <v>2.1</v>
+      </c>
+      <c r="F57">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1000000</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>3.01</v>
+      </c>
+      <c r="D58">
+        <v>2.16</v>
+      </c>
+      <c r="E58">
+        <v>1.98</v>
+      </c>
+      <c r="F58">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1000000</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <v>2.81</v>
+      </c>
+      <c r="D59">
+        <v>2.04</v>
+      </c>
+      <c r="E59">
+        <v>1.9</v>
+      </c>
+      <c r="F59">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="1">
+        <f>AVERAGE(C57:C59)</f>
+        <v>2.9433333333333334</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" ref="D60:F60" si="45">AVERAGE(D57:D59)</f>
+        <v>2.1466666666666669</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="45"/>
+        <v>1.9933333333333334</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="45"/>
+        <v>1.2733333333333334</v>
+      </c>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="1">
+        <f>STDEV(C57:C59)</f>
+        <v>0.115470053837925</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" ref="D61:F61" si="46">STDEV(D57:D59)</f>
+        <v>0.10066445913694343</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="46"/>
+        <v>0.10066445913694343</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="46"/>
+        <v>6.1101009266077921E-2</v>
+      </c>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>10000000</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>25.32</v>
+      </c>
+      <c r="D62">
+        <v>21.95</v>
+      </c>
+      <c r="E62">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="F62">
+        <v>12.46</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>10000000</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>27.69</v>
+      </c>
+      <c r="D63">
+        <v>20.260000000000002</v>
+      </c>
+      <c r="E63">
+        <v>20.85</v>
+      </c>
+      <c r="F63">
+        <v>12.69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>10000000</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64">
+        <v>25.18</v>
+      </c>
+      <c r="D64">
+        <v>21.69</v>
+      </c>
+      <c r="E64">
+        <v>19.690000000000001</v>
+      </c>
+      <c r="F64">
+        <v>12.35</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="1">
+        <f>AVERAGE(C62:C64)</f>
+        <v>26.063333333333333</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" ref="D65:F65" si="47">AVERAGE(D62:D64)</f>
+        <v>21.3</v>
+      </c>
+      <c r="E65" s="1">
+        <f t="shared" si="47"/>
+        <v>20.070000000000004</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="47"/>
+        <v>12.5</v>
+      </c>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B66" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="1">
+        <f>STDEV(C62:C64)</f>
+        <v>1.4104727339914571</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" ref="D66:F66" si="48">STDEV(D62:D64)</f>
+        <v>0.90999999999999903</v>
+      </c>
+      <c r="E66" s="1">
+        <f t="shared" si="48"/>
+        <v>0.67557383016218142</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" si="48"/>
+        <v>0.17349351572897451</v>
+      </c>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82CA933-4B9D-F74D-AC6C-F94BD887C138}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" zoomScale="125" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.84</v>
+      </c>
+      <c r="B2">
+        <v>5.6733333333333329</v>
+      </c>
+      <c r="C2">
+        <v>41.593333333333334</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>A$2/($D2*A2)</f>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:H5" si="0">B$2/($D2*B2)</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.47333333333333333</v>
+      </c>
+      <c r="B3">
+        <v>3.18</v>
+      </c>
+      <c r="C3">
+        <v>24.926666666666666</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F5" si="1">A$2/($D3*A3)</f>
+        <v>0.88732394366197176</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>0.89203354297693904</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>0.8343139876972453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="B4">
+        <v>2.1233333333333335</v>
+      </c>
+      <c r="C4">
+        <v>19.63</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.72413793103448276</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.66797488226059643</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.52971642044489731</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.29333333333333328</v>
+      </c>
+      <c r="B5">
+        <v>2.1366666666666667</v>
+      </c>
+      <c r="C5">
+        <v>21.243333333333336</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.35795454545454553</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.3319032761310452</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.24474344892515296</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2.9433333333333334</v>
+      </c>
+      <c r="B28">
+        <v>26.063333333333333</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f>A$28/($D28*A28)</f>
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f>B$28/($D28*B28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2.1466666666666669</v>
+      </c>
+      <c r="B29">
+        <v>21.3</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29:F31" si="2">A$28/($D29*A29)</f>
+        <v>0.68555900621118004</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:G31" si="3">B$28/($D29*B29)</f>
+        <v>0.61181533646322372</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1.9933333333333334</v>
+      </c>
+      <c r="B30">
+        <v>20.070000000000004</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>0.36914715719063546</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>0.3246553728616508</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1.2733333333333334</v>
+      </c>
+      <c r="B31">
+        <v>12.5</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>0.28893979057591623</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>0.26063333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>